<commit_message>
Jo's edits to ch1. Consistent capitalization to ch1.
</commit_message>
<xml_diff>
--- a/data/Extended/ReciprocityCheck/ReciprocityCheck.xlsx
+++ b/data/Extended/ReciprocityCheck/ReciprocityCheck.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Period</t>
   </si>
@@ -58,16 +58,47 @@
   </si>
   <si>
     <t>Original situation:</t>
+  </si>
+  <si>
+    <t>Original command:</t>
+  </si>
+  <si>
+    <t>./pegSerial --mode constantIncidence --min 410 --max 410 --increment 1 --incidenceAngle 88 --outputFile reciprocityOutput.txt --gratingType blazed --gratingPeriod 1 --gratingMaterial Pt --N 15 --gratingGeometry 2.5,30 --eV</t>
+  </si>
+  <si>
+    <t>Reciprocity command:</t>
+  </si>
+  <si>
+    <t>./pegSerial --mode constantIncidence --min 410 --max 410 --increment 1 --incidenceAngle -85.11446088 --outputFile reciprocityOutput.txt --gratingType blazed --gratingPeriod 1 --gratingMaterial Pt --N 15 --gratingGeometry 2.5,30 --eV</t>
+  </si>
+  <si>
+    <t>Or, instead of negative incidence, can mirror the grating geometry:</t>
+  </si>
+  <si>
+    <t>./pegSerial --mode constantIncidence --min 410 --max 410 --increment 1 --incidenceAngle 85.11446088 --outputFile reciprocityOutput.txt --gratingType blazed --gratingPeriod 1 --gratingMaterial Pt --N 15 --gratingGeometry 30,2.5 --eV</t>
+  </si>
+  <si>
+    <t>Flipping the geometry to check if 0 order at 88 deg. Incidence remains constant for (2.5,30) and (30,2.5) blaze gratings:</t>
+  </si>
+  <si>
+    <t>./pegSerial --mode constantIncidence --min 410 --max 410 --increment 1 --incidenceAngle 88 --outputFile reciprocityOutput.txt --gratingType blazed --gratingPeriod 1 --gratingMaterial Pt --N 15 --gratingGeometry 30,2.5 --eV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,6 +127,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -112,12 +151,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -169,43 +213,76 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="14">
-    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
+  <cellStyles count="29">
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="2" builtinId="21"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -534,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -545,7 +622,7 @@
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -553,7 +630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -573,7 +650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -593,7 +670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -615,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:32">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -635,7 +712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:32">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -656,7 +733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:32">
       <c r="B8" s="2">
         <f>B7*PI()/180</f>
         <v>1.5358897417550099</v>
@@ -672,7 +749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:32">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -694,7 +771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:32">
       <c r="B11" s="3">
         <f>B10*180/PI()</f>
         <v>85.114460875075764</v>
@@ -708,6 +785,494 @@
       </c>
       <c r="H11" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="B13">
+        <v>-15</v>
+      </c>
+      <c r="C13">
+        <v>-14</v>
+      </c>
+      <c r="D13">
+        <v>-13</v>
+      </c>
+      <c r="E13">
+        <v>-12</v>
+      </c>
+      <c r="F13">
+        <v>-11</v>
+      </c>
+      <c r="G13">
+        <v>-10</v>
+      </c>
+      <c r="H13">
+        <v>-9</v>
+      </c>
+      <c r="I13">
+        <v>-8</v>
+      </c>
+      <c r="J13">
+        <v>-7</v>
+      </c>
+      <c r="K13">
+        <v>-6</v>
+      </c>
+      <c r="L13">
+        <v>-5</v>
+      </c>
+      <c r="M13">
+        <v>-4</v>
+      </c>
+      <c r="N13">
+        <v>-3</v>
+      </c>
+      <c r="O13">
+        <v>-2</v>
+      </c>
+      <c r="P13">
+        <v>-1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32">
+      <c r="A16" s="4">
+        <v>410</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1.9282900000000001E-5</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1.4587799999999999E-5</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1.9555099999999998E-5</v>
+      </c>
+      <c r="E16" s="5">
+        <v>5.0599700000000003E-5</v>
+      </c>
+      <c r="F16" s="5">
+        <v>4.8336700000000001E-5</v>
+      </c>
+      <c r="G16" s="5">
+        <v>4.3492299999999997E-5</v>
+      </c>
+      <c r="H16">
+        <v>1.8980900000000001E-4</v>
+      </c>
+      <c r="I16">
+        <v>1.4251199999999999E-4</v>
+      </c>
+      <c r="J16">
+        <v>3.4380899999999999E-4</v>
+      </c>
+      <c r="K16">
+        <v>1.2322100000000001E-3</v>
+      </c>
+      <c r="L16">
+        <v>7.9432400000000001E-4</v>
+      </c>
+      <c r="M16">
+        <v>1.34339E-2</v>
+      </c>
+      <c r="N16">
+        <v>7.2255E-2</v>
+      </c>
+      <c r="O16">
+        <v>9.8549200000000003E-2</v>
+      </c>
+      <c r="P16" s="4">
+        <v>8.2351900000000006E-2</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>0.18124499999999999</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32">
+      <c r="A21">
+        <v>410</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" s="4">
+        <v>8.2333900000000002E-2</v>
+      </c>
+      <c r="Q21">
+        <v>5.91269E-3</v>
+      </c>
+      <c r="R21">
+        <v>1.96715E-3</v>
+      </c>
+      <c r="S21">
+        <v>8.1469300000000001E-4</v>
+      </c>
+      <c r="T21">
+        <v>3.9588299999999998E-4</v>
+      </c>
+      <c r="U21">
+        <v>2.1619900000000001E-4</v>
+      </c>
+      <c r="V21" s="5">
+        <v>1.2651599999999999E-4</v>
+      </c>
+      <c r="W21" s="5">
+        <v>7.87885E-5</v>
+      </c>
+      <c r="X21" s="5">
+        <v>5.2108899999999998E-5</v>
+      </c>
+      <c r="Y21" s="5">
+        <v>3.8543300000000001E-5</v>
+      </c>
+      <c r="Z21" s="5">
+        <v>3.0259700000000001E-5</v>
+      </c>
+      <c r="AA21" s="5">
+        <v>2.3973700000000001E-5</v>
+      </c>
+      <c r="AB21" s="5">
+        <v>1.9278499999999998E-5</v>
+      </c>
+      <c r="AC21" s="5">
+        <v>1.4967700000000001E-5</v>
+      </c>
+      <c r="AD21" s="5">
+        <v>1.3452799999999999E-5</v>
+      </c>
+      <c r="AE21" s="5">
+        <v>1.16629E-5</v>
+      </c>
+      <c r="AF21" s="5">
+        <v>6.8690800000000003E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32">
+      <c r="A25">
+        <v>410</v>
+      </c>
+      <c r="B25" s="5">
+        <v>6.8690800000000003E-6</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1.16629E-5</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1.3452799999999999E-5</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1.4967700000000001E-5</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1.9278499999999998E-5</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2.3973700000000001E-5</v>
+      </c>
+      <c r="H25" s="5">
+        <v>3.0259700000000001E-5</v>
+      </c>
+      <c r="I25" s="5">
+        <v>3.8543300000000001E-5</v>
+      </c>
+      <c r="J25" s="5">
+        <v>5.2108899999999998E-5</v>
+      </c>
+      <c r="K25" s="5">
+        <v>7.87885E-5</v>
+      </c>
+      <c r="L25">
+        <v>1.2651599999999999E-4</v>
+      </c>
+      <c r="M25">
+        <v>2.1619900000000001E-4</v>
+      </c>
+      <c r="N25">
+        <v>3.9588299999999998E-4</v>
+      </c>
+      <c r="O25">
+        <v>8.1469300000000001E-4</v>
+      </c>
+      <c r="P25">
+        <v>1.96715E-3</v>
+      </c>
+      <c r="Q25">
+        <v>5.91269E-3</v>
+      </c>
+      <c r="R25" s="4">
+        <v>8.2333900000000002E-2</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32">
+      <c r="A30">
+        <v>410</v>
+      </c>
+      <c r="B30" s="5">
+        <v>3.1239699999999998E-5</v>
+      </c>
+      <c r="C30" s="5">
+        <v>3.3594799999999999E-5</v>
+      </c>
+      <c r="D30" s="5">
+        <v>4.0961999999999998E-5</v>
+      </c>
+      <c r="E30" s="5">
+        <v>5.5409799999999999E-5</v>
+      </c>
+      <c r="F30" s="5">
+        <v>6.7966000000000006E-5</v>
+      </c>
+      <c r="G30" s="5">
+        <v>8.9053600000000004E-5</v>
+      </c>
+      <c r="H30">
+        <v>1.20155E-4</v>
+      </c>
+      <c r="I30">
+        <v>1.6152500000000001E-4</v>
+      </c>
+      <c r="J30">
+        <v>2.4344500000000001E-4</v>
+      </c>
+      <c r="K30">
+        <v>3.8203299999999999E-4</v>
+      </c>
+      <c r="L30">
+        <v>6.4869400000000001E-4</v>
+      </c>
+      <c r="M30">
+        <v>1.22046E-3</v>
+      </c>
+      <c r="N30">
+        <v>2.6159600000000001E-3</v>
+      </c>
+      <c r="O30">
+        <v>6.6307400000000004E-3</v>
+      </c>
+      <c r="P30">
+        <v>2.086E-2</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>0.18124499999999999</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <v>0</v>
+      </c>
+      <c r="AB30">
+        <v>0</v>
+      </c>
+      <c r="AC30">
+        <v>0</v>
+      </c>
+      <c r="AD30">
+        <v>0</v>
+      </c>
+      <c r="AE30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>